<commit_message>
Add pairwise test tables
</commit_message>
<xml_diff>
--- a/Tables/Beta_group_significance_Family_Tribe.xlsx
+++ b/Tables/Beta_group_significance_Family_Tribe.xlsx
@@ -29,10 +29,10 @@
       <b val="1"/>
     </font>
     <font>
-      <color rgb="00000000"/>
+      <color rgb="00FF0000"/>
     </font>
     <font>
-      <color rgb="00FF0000"/>
+      <color rgb="00000000"/>
     </font>
   </fonts>
   <fills count="2">
@@ -366,7 +366,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -387,20 +387,30 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>Sample size</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Permutations</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>pseudo-F</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>p-value</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>q-value</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
@@ -409,24 +419,30 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A (n=5)</t>
+          <t>Cyprinidae</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>J (n=27)</t>
+          <t>Nemacheilidae</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6.077441077441094</v>
+        <v>82</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01369189616538225</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>0.09348600311378276</v>
-      </c>
-      <c r="F2" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5.488551516114762</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>0.003333333333333333</v>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>skin</t>
         </is>
@@ -435,24 +451,30 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>A (n=5)</t>
+          <t>Haplochrominae</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>S (n=35)</t>
+          <t>Nemacheilidae</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>5.529616724738673</v>
+        <v>21</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01869720062275656</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>0.09348600311378276</v>
-      </c>
-      <c r="F3" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.797867053529889</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>0.003333333333333333</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>skin</t>
         </is>
@@ -461,24 +483,30 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>A (n=5)</t>
+          <t>Nemacheilidae</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>H (n=27)</t>
+          <t>Tilapiinae</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3.394612794612783</v>
+        <v>30</v>
       </c>
       <c r="D4" t="n">
-        <v>0.06540971903742436</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>0.1635242975935609</v>
-      </c>
-      <c r="F4" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5.118943530524485</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>0.003333333333333333</v>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>skin</t>
         </is>
@@ -487,24 +515,30 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>H (n=27)</t>
+          <t>Cyprinidae</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>J (n=27)</t>
+          <t>Tilapiinae</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3.855518144407029</v>
+        <v>76</v>
       </c>
       <c r="D5" t="n">
-        <v>0.04958260976434615</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0.1635242975935609</v>
-      </c>
-      <c r="F5" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2.200512011144967</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>0.0275</v>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>skin</t>
         </is>
@@ -513,24 +547,30 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>J (n=27)</t>
+          <t>Cyprinidae</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>T (n=4)</t>
+          <t>Haplochrominae</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2.722222222222229</v>
+        <v>67</v>
       </c>
       <c r="D6" t="n">
-        <v>0.09896015401940557</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0.1979203080388111</v>
-      </c>
-      <c r="F6" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.674086943068863</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.047</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>skin</t>
         </is>
@@ -539,24 +579,30 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>S (n=35)</t>
+          <t>Mugilidae</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>T (n=4)</t>
+          <t>Nemacheilidae</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.928571428571445</v>
+        <v>19</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1649148225532956</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>0.274858037588826</v>
-      </c>
-      <c r="F7" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.574511583218658</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>skin</t>
         </is>
@@ -565,24 +611,30 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>H (n=27)</t>
+          <t>Cyprinidae</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>S (n=35)</t>
+          <t>Mugilidae</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.687528344671222</v>
+        <v>65</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1939271084299195</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>0.2770387263284564</v>
-      </c>
-      <c r="F8" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.41020188514425</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>0.1657142857142857</v>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>skin</t>
         </is>
@@ -591,24 +643,30 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>H (n=27)</t>
+          <t>Mugilidae</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>T (n=4)</t>
+          <t>Tilapiinae</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.003472222222214</v>
+        <v>13</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3164717878479773</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>0.3955897348099716</v>
-      </c>
-      <c r="F9" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.01936922172975</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.4379999999999999</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>0.5475</v>
+      </c>
+      <c r="H9" t="inlineStr">
         <is>
           <t>skin</t>
         </is>
@@ -617,24 +675,30 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>A (n=5)</t>
+          <t>Haplochrominae</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>T (n=4)</t>
+          <t>Tilapiinae</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.5400000000000027</v>
+        <v>15</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4624327264504752</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>0.5091431693941095</v>
-      </c>
-      <c r="F10" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.8030617216277397</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>0.7666666666666666</v>
+      </c>
+      <c r="H10" t="inlineStr">
         <is>
           <t>skin</t>
         </is>
@@ -643,24 +707,30 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>J (n=27)</t>
+          <t>Haplochrominae</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>S (n=35)</t>
+          <t>Mugilidae</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.4358276643990848</v>
+        <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5091431693941095</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>0.5091431693941095</v>
-      </c>
-      <c r="F11" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.5317967231327185</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="inlineStr">
         <is>
           <t>skin</t>
         </is>
@@ -669,24 +739,30 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>A (n=18)</t>
+          <t>Cyprinidae</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>H (n=27)</t>
+          <t>Haplochrominae</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>30.14975845410627</v>
+        <v>72</v>
       </c>
       <c r="D12" t="n">
-        <v>3.999369967013239e-08</v>
-      </c>
-      <c r="E12" s="3" t="n">
-        <v>3.999369967013239e-07</v>
-      </c>
-      <c r="F12" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4.176275092303046</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>0.0025</v>
+      </c>
+      <c r="H12" t="inlineStr">
         <is>
           <t>swab</t>
         </is>
@@ -695,24 +771,30 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>A (n=18)</t>
+          <t>Cyprinidae</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>J (n=29)</t>
+          <t>Mugilidae</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>26.00047892720307</v>
+        <v>67</v>
       </c>
       <c r="D13" t="n">
-        <v>3.41332671921846e-07</v>
-      </c>
-      <c r="E13" s="3" t="n">
-        <v>1.195329918280768e-06</v>
-      </c>
-      <c r="F13" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.68038110964364</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>0.0025</v>
+      </c>
+      <c r="H13" t="inlineStr">
         <is>
           <t>swab</t>
         </is>
@@ -721,24 +803,30 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>H (n=27)</t>
+          <t>Cyprinidae</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>S (n=35)</t>
+          <t>Nemacheilidae</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>25.90521541950116</v>
+        <v>85</v>
       </c>
       <c r="D14" t="n">
-        <v>3.585989754842305e-07</v>
-      </c>
-      <c r="E14" s="3" t="n">
-        <v>1.195329918280768e-06</v>
-      </c>
-      <c r="F14" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.271030444259854</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>0.0025</v>
+      </c>
+      <c r="H14" t="inlineStr">
         <is>
           <t>swab</t>
         </is>
@@ -747,24 +835,30 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>A (n=18)</t>
+          <t>Cyprinidae</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>S (n=35)</t>
+          <t>Tilapiinae</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>15.1142857142857</v>
+        <v>86</v>
       </c>
       <c r="D15" t="n">
-        <v>0.000101194605245838</v>
-      </c>
-      <c r="E15" s="3" t="n">
-        <v>0.0002529865131145949</v>
-      </c>
-      <c r="F15" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E15" t="n">
+        <v>5.601916698492269</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>0.0025</v>
+      </c>
+      <c r="H15" t="inlineStr">
         <is>
           <t>swab</t>
         </is>
@@ -773,24 +867,30 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>H (n=27)</t>
+          <t>Haplochrominae</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>T (n=11)</t>
+          <t>Nemacheilidae</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>13.11188811188811</v>
+        <v>29</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0002934278077338205</v>
-      </c>
-      <c r="E16" s="3" t="n">
-        <v>0.000586855615467641</v>
-      </c>
-      <c r="F16" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E16" t="n">
+        <v>4.176009284009917</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>0.0025</v>
+      </c>
+      <c r="H16" t="inlineStr">
         <is>
           <t>swab</t>
         </is>
@@ -799,24 +899,30 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>A (n=18)</t>
+          <t>Nemacheilidae</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>T (n=11)</t>
+          <t>Tilapiinae</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>10.47272727272727</v>
+        <v>43</v>
       </c>
       <c r="D17" t="n">
-        <v>0.00121149736543063</v>
-      </c>
-      <c r="E17" s="3" t="n">
-        <v>0.002019162275717717</v>
-      </c>
-      <c r="F17" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4.666365324523966</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>0.0025</v>
+      </c>
+      <c r="H17" t="inlineStr">
         <is>
           <t>swab</t>
         </is>
@@ -825,24 +931,30 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>H (n=27)</t>
+          <t>Cyprinidae</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>J (n=29)</t>
+          <t>Poeciliidae</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>9.452510586811854</v>
+        <v>66</v>
       </c>
       <c r="D18" t="n">
-        <v>0.002108602811171743</v>
-      </c>
-      <c r="E18" s="3" t="n">
-        <v>0.003012289730245348</v>
-      </c>
-      <c r="F18" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2.190419581752153</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>0.004285714285714286</v>
+      </c>
+      <c r="H18" t="inlineStr">
         <is>
           <t>swab</t>
         </is>
@@ -851,24 +963,30 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>J (n=29)</t>
+          <t>Mugilidae</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>S (n=35)</t>
+          <t>Nemacheilidae</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>7.681136794240245</v>
+        <v>24</v>
       </c>
       <c r="D19" t="n">
-        <v>0.005580100546048133</v>
-      </c>
-      <c r="E19" s="3" t="n">
-        <v>0.006975125682560166</v>
-      </c>
-      <c r="F19" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2.912168279401778</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.006999999999999999</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>0.013125</v>
+      </c>
+      <c r="H19" t="inlineStr">
         <is>
           <t>swab</t>
         </is>
@@ -877,24 +995,30 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>J (n=29)</t>
+          <t>Nemacheilidae</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>T (n=11)</t>
+          <t>Poeciliidae</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3.699594770242385</v>
+        <v>23</v>
       </c>
       <c r="D20" t="n">
-        <v>0.05442568464899194</v>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>0.06047298294332438</v>
-      </c>
-      <c r="F20" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2.37651549592365</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>0.02666666666666667</v>
+      </c>
+      <c r="H20" t="inlineStr">
         <is>
           <t>swab</t>
         </is>
@@ -903,24 +1027,190 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>S (n=35)</t>
+          <t>Mugilidae</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>T (n=11)</t>
+          <t>Poeciliidae</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.04791378833931503</v>
+        <v>5</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8267340348832932</v>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>0.8267340348832932</v>
-      </c>
-      <c r="F21" t="inlineStr">
+        <v>999</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1.412334598498102</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.124</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>0.186</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>swab</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Haplochrominae</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Poeciliidae</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>10</v>
+      </c>
+      <c r="D22" t="n">
+        <v>999</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1.062315513686372</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.309</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>0.38625</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>swab</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Mugilidae</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Tilapiinae</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>25</v>
+      </c>
+      <c r="D23" t="n">
+        <v>999</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1.106679514838405</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G23" s="3" t="n">
+        <v>0.38625</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>swab</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Poeciliidae</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Tilapiinae</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>24</v>
+      </c>
+      <c r="D24" t="n">
+        <v>999</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1.065764123709873</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.353</v>
+      </c>
+      <c r="G24" s="3" t="n">
+        <v>0.4073076923076923</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>swab</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Haplochrominae</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Mugilidae</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>11</v>
+      </c>
+      <c r="D25" t="n">
+        <v>999</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.9889175056798988</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.421</v>
+      </c>
+      <c r="G25" s="3" t="n">
+        <v>0.4510714285714286</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>swab</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Haplochrominae</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Tilapiinae</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>30</v>
+      </c>
+      <c r="D26" t="n">
+        <v>999</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.8057155740773592</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.711</v>
+      </c>
+      <c r="G26" s="3" t="n">
+        <v>0.711</v>
+      </c>
+      <c r="H26" t="inlineStr">
         <is>
           <t>swab</t>
         </is>

</xml_diff>